<commit_message>
Built site for MassWateR: 1.0.0.9000@123d66b
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49316AFF-31BD-4148-80AA-FA0E527BE58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC22C19-9F5D-4BFF-A9E2-358556A614C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>Sampling depth unit of measure.</t>
-  </si>
-  <si>
-    <t>Name of the measured parameter.</t>
   </si>
   <si>
     <t>value, BDL, AQL</t>
@@ -406,92 +403,96 @@
     <t>If the Result Value is BDL or AQL, this column will be checked for the limit value.  If a value is entered here it will be used.  Otherwise, the value in the MDL or UQL column in the DQO Accuracy file will be used.  MassWateR analytical functions will use 1/2 of the MDL and 100% of the UQL.</t>
   </si>
   <si>
-    <t>Optional field that can be used to group results using whatever coding system the users wants, such as wet weather or dry weather.
+    <t>The Results tab must be the first tab in this workbook.</t>
+  </si>
+  <si>
+    <t>Sampling Date (formatted as date in Exel M/D/YYYY)</t>
+  </si>
+  <si>
+    <t>ft, m</t>
+  </si>
+  <si>
+    <t>Surface, Bottom, Midwater, Near Bottom</t>
+  </si>
+  <si>
+    <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.</t>
+  </si>
+  <si>
+    <t>Either Depth or Relative Depth is required.  Relative Depth is a description of the relative depth in the water body, such as "Surface" or "Bottom".  MassWateR analytical functions only evaluate surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
+  </si>
+  <si>
+    <t>Sampling Depth.  MassWateR analytical functions only evaluate surface samples.  It considers all samples &lt; 1 m or &lt; 3.3 ft to be surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
+  </si>
+  <si>
+    <t>Required?</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Either Depth or Relative Depth Required for non-QC entries</t>
+  </si>
+  <si>
+    <t>Required for non-QC entries</t>
+  </si>
+  <si>
+    <t>Required if Depth entered</t>
+  </si>
+  <si>
+    <t>Only for duplicates, spikes, and instrument checks</t>
+  </si>
+  <si>
+    <t>As needed</t>
+  </si>
+  <si>
+    <t>Leave cells blank if they are not required and they don't need a value.</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Sample Collection Method ID</t>
+  </si>
+  <si>
+    <t>Grab</t>
+  </si>
+  <si>
+    <t>Result Comment</t>
+  </si>
+  <si>
+    <t>Water Quality</t>
+  </si>
+  <si>
+    <t>River was very full</t>
+  </si>
+  <si>
+    <t>defined in WQX by organization</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the method ID used for this sample collection.  Method IDs are defined in WQX by organization.  Not applicable for field measurement/observations.  MassWateR will assign a default value of "Grab" if nothing is entered.</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the Project ID as defined in WQX.  MassWateR will assign a default value of "Water Quality" if nothing is entered.</t>
+  </si>
+  <si>
+    <t>Required for activity type Sample-Routine only</t>
+  </si>
+  <si>
+    <t>Free-form comments about the sample.</t>
+  </si>
+  <si>
+    <t>any note</t>
+  </si>
+  <si>
+    <t>Name of the measured parameter.
+- Note that this can be either the WQX or Simple parameter name.  However, if a parameter is distinguished by Sample Fraction only (i.e. TDP, PON, TDN), then the Simple parameter name must be used here and in all other files (WQX, DQO, etc.).</t>
+  </si>
+  <si>
+    <t>Optional (for analysis) field that can be used to group results using whatever coding system the users wants, such as wet weather or dry weather.
 This field can also be used to record sample IDs for QC samples, such as lab blanks and lab dulicates.</t>
-  </si>
-  <si>
-    <t>The Results tab must be the first tab in this workbook.</t>
-  </si>
-  <si>
-    <t>Sampling Date (formatted as date in Exel M/D/YYYY)</t>
-  </si>
-  <si>
-    <t>ft, m</t>
-  </si>
-  <si>
-    <t>Surface, Bottom, Midwater, Near Bottom</t>
-  </si>
-  <si>
-    <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.</t>
-  </si>
-  <si>
-    <t>Either Depth or Relative Depth is required.  Relative Depth is a description of the relative depth in the water body, such as "Surface" or "Bottom".  MassWateR analytical functions only evaluate surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
-  </si>
-  <si>
-    <t>Sampling Depth.  MassWateR analytical functions only evaluate surface samples.  It considers all samples &lt; 1 m or &lt; 3.3 ft to be surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
-  </si>
-  <si>
-    <t>Required?</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Either Depth or Relative Depth Required for non-QC entries</t>
-  </si>
-  <si>
-    <t>Required for non-QC entries</t>
-  </si>
-  <si>
-    <t>Required if Depth entered</t>
-  </si>
-  <si>
-    <t>Only for duplicates, spikes, and instrument checks</t>
-  </si>
-  <si>
-    <t>As needed</t>
-  </si>
-  <si>
-    <t>Leave cells blank if they are not required and they don't need a value.</t>
-  </si>
-  <si>
-    <t>Project ID</t>
-  </si>
-  <si>
-    <t>Sample Collection Method ID</t>
-  </si>
-  <si>
-    <t>Grab</t>
-  </si>
-  <si>
-    <t>Result Comment</t>
-  </si>
-  <si>
-    <t>Water Quality</t>
-  </si>
-  <si>
-    <t>River was very full</t>
-  </si>
-  <si>
-    <t>defined in WQX by organization</t>
-  </si>
-  <si>
-    <t>For WQX:  Enter the method ID used for this sample collection.  Method IDs are defined in WQX by organization.  Not applicable for field measurement/observations.  MassWateR will assign a default value of "Grab" if nothing is entered.</t>
-  </si>
-  <si>
-    <t>For WQX:  Enter the Project ID as defined in WQX.  MassWateR will assign a default value of "Water Quality" if nothing is entered.</t>
-  </si>
-  <si>
-    <t>Required for activity type Sample-Routine only</t>
-  </si>
-  <si>
-    <t>Free-form comments about the sample.</t>
-  </si>
-  <si>
-    <t>any note</t>
   </si>
 </sst>
 </file>
@@ -1029,25 +1030,25 @@
       <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="5"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1091,16 +1092,16 @@
         <v>24</v>
       </c>
       <c r="O1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1135,10 +1136,10 @@
         <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1170,16 +1171,16 @@
         <v>12</v>
       </c>
       <c r="O3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" t="s">
         <v>73</v>
       </c>
-      <c r="P3" t="s">
-        <v>75</v>
-      </c>
       <c r="Q3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1205,10 +1206,10 @@
         <v>34</v>
       </c>
       <c r="P4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1254,34 +1255,34 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="96.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="24" customWidth="1"/>
+    <col min="1" max="1" width="30.26953125" customWidth="1"/>
+    <col min="2" max="2" width="96.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>36</v>
       </c>
@@ -1295,10 +1296,10 @@
         <v>40</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
@@ -1312,15 +1313,15 @@
         <v>43</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>14</v>
@@ -1329,55 +1330,55 @@
         <v>42</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="18">
         <v>44383</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="19">
         <v>0.24652777777777801</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="17">
         <v>0.75</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
@@ -1388,35 +1389,35 @@
         <v>11</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
@@ -1425,32 +1426,32 @@
         <v>41</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="17">
         <v>810</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1459,40 +1460,40 @@
         <v>41</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="17">
         <v>1500</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="17">
         <v>830</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
@@ -1503,18 +1504,18 @@
         <v>16</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
@@ -1523,56 +1524,56 @@
         <v>43</v>
       </c>
       <c r="E19" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="B21" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="25" t="s">
+      <c r="B22" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@caa7157
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC22C19-9F5D-4BFF-A9E2-358556A614C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F25540B-3B8D-438B-95F4-F28406E89D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -472,9 +472,6 @@
     <t>defined in WQX by organization</t>
   </si>
   <si>
-    <t>For WQX:  Enter the method ID used for this sample collection.  Method IDs are defined in WQX by organization.  Not applicable for field measurement/observations.  MassWateR will assign a default value of "Grab" if nothing is entered.</t>
-  </si>
-  <si>
     <t>For WQX:  Enter the Project ID as defined in WQX.  MassWateR will assign a default value of "Water Quality" if nothing is entered.</t>
   </si>
   <si>
@@ -493,6 +490,9 @@
   <si>
     <t>Optional (for analysis) field that can be used to group results using whatever coding system the users wants, such as wet weather or dry weather.
 This field can also be used to record sample IDs for QC samples, such as lab blanks and lab dulicates.</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the method ID used for this sample collection.  Method IDs are defined in WQX by organization.  Not applicable for field measurement/observations.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassBays" in the WQXMeta file.</t>
   </si>
 </sst>
 </file>
@@ -1023,32 +1023,32 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="5"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" customWidth="1"/>
-    <col min="17" max="17" width="12.1796875" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -1251,38 +1251,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78C6628-51AC-4A46-96D9-F2FA0EFA1B4C}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="2" width="96.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.1796875" style="24" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="96.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>36</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>4</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>25</v>
       </c>
@@ -1412,12 +1412,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
@@ -1429,7 +1429,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
@@ -1510,12 +1510,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
@@ -1527,12 +1527,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>71</v>
@@ -1541,15 +1541,15 @@
         <v>75</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>73</v>
@@ -1561,15 +1561,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@443157d
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F25540B-3B8D-438B-95F4-F28406E89D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6F3B8-41A7-4627-A593-09E952C2B573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -415,9 +415,6 @@
     <t>Surface, Bottom, Midwater, Near Bottom</t>
   </si>
   <si>
-    <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.</t>
-  </si>
-  <si>
     <t>Either Depth or Relative Depth is required.  Relative Depth is a description of the relative depth in the water body, such as "Surface" or "Bottom".  MassWateR analytical functions only evaluate surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
   </si>
   <si>
@@ -493,6 +490,10 @@
   </si>
   <si>
     <t>For WQX:  Enter the method ID used for this sample collection.  Method IDs are defined in WQX by organization.  Not applicable for field measurement/observations.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassBays" in the WQXMeta file.</t>
+  </si>
+  <si>
+    <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.
+- One exception to this rule is Lab Spikes.  Lab Spikes may be entered for any parameter with a % unit of measure.  "% recovery" is recommended but "%" can also be used.</t>
   </si>
 </sst>
 </file>
@@ -1092,13 +1093,13 @@
         <v>24</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1136,7 +1137,7 @@
         <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1171,13 +1172,13 @@
         <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" t="s">
         <v>73</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1206,7 +1207,7 @@
         <v>34</v>
       </c>
       <c r="P4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1232,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1279,7 +1280,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1296,7 +1297,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1313,7 +1314,7 @@
         <v>43</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="225" x14ac:dyDescent="0.25">
@@ -1330,7 +1331,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1345,7 +1346,7 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1361,7 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1368,14 +1369,14 @@
         <v>4</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="17">
         <v>0.75</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,7 +1393,7 @@
         <v>55</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1400,7 +1401,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>23</v>
@@ -1409,7 +1410,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1417,7 +1418,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
@@ -1426,7 +1427,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1443,15 +1444,15 @@
         <v>46</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1460,7 +1461,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1475,7 +1476,7 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1490,7 +1491,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1507,7 +1508,7 @@
         <v>48</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1515,7 +1516,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
@@ -1524,56 +1525,56 @@
         <v>43</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="D20" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@3a0ad8b
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6F3B8-41A7-4627-A593-09E952C2B573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E57C3B6-0A16-4A4B-B736-68041709BC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -489,11 +489,11 @@
 This field can also be used to record sample IDs for QC samples, such as lab blanks and lab dulicates.</t>
   </si>
   <si>
-    <t>For WQX:  Enter the method ID used for this sample collection.  Method IDs are defined in WQX by organization.  Not applicable for field measurement/observations.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassBays" in the WQXMeta file.</t>
-  </si>
-  <si>
     <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.
 - One exception to this rule is Lab Spikes.  Lab Spikes may be entered for any parameter with a % unit of measure.  "% recovery" is recommended but "%" can also be used.</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab", "Pole", and "Basket".</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:Q1"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1256,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1452,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1528,12 +1528,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@a1f6b61
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3105B2BE-C6EE-4AAE-9C16-DC6A4B2172C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE51E64-D386-4FF2-B8DB-5DD9DE790D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>cfu/100ml</t>
   </si>
   <si>
-    <t>Quality Control Field Calibration Check</t>
-  </si>
-  <si>
     <t>K16452-MB3</t>
   </si>
   <si>
@@ -205,6 +202,122 @@
   </si>
   <si>
     <t>see parameter list</t>
+  </si>
+  <si>
+    <t>user defined</t>
+  </si>
+  <si>
+    <t>Qualification code for samples.  Leave blank for samples that are considered good without question.  Enter "Q" for samples that have been identified as questionable.  Censored samples should not be entered at all.</t>
+  </si>
+  <si>
+    <t>Sampling depth unit of measure.</t>
+  </si>
+  <si>
+    <t>value, BDL, AQL</t>
+  </si>
+  <si>
+    <t>This is used for duplicates, spikes, and calibration checks.  For duplicates, the second value is entered here.  For spikes, the reference target is entered here.  For calibration checks, the target calibration standard is entered here.</t>
+  </si>
+  <si>
+    <t>blank, Q</t>
+  </si>
+  <si>
+    <t>Sampling Time (formatted as time in Excel with correct AM/PM)</t>
+  </si>
+  <si>
+    <t>Numeric measured value.  If the value is below the detection limit, enter "BDL".  If the value is above the quantitation limit, enter "AQL".</t>
+  </si>
+  <si>
+    <t>If the Result Value is BDL or AQL, this column will be checked for the limit value.  If a value is entered here it will be used.  Otherwise, the value in the MDL or UQL column in the DQO Accuracy file will be used.  MassWateR analytical functions will use 1/2 of the MDL and 100% of the UQL.</t>
+  </si>
+  <si>
+    <t>The Results tab must be the first tab in this workbook.</t>
+  </si>
+  <si>
+    <t>Sampling Date (formatted as date in Exel M/D/YYYY)</t>
+  </si>
+  <si>
+    <t>ft, m</t>
+  </si>
+  <si>
+    <t>Surface, Bottom, Midwater, Near Bottom</t>
+  </si>
+  <si>
+    <t>Either Depth or Relative Depth is required.  Relative Depth is a description of the relative depth in the water body, such as "Surface" or "Bottom".  MassWateR analytical functions only evaluate surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
+  </si>
+  <si>
+    <t>Sampling Depth.  MassWateR analytical functions only evaluate surface samples.  It considers all samples &lt; 1 m or &lt; 3.3 ft to be surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
+  </si>
+  <si>
+    <t>Required?</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Either Depth or Relative Depth Required for non-QC entries</t>
+  </si>
+  <si>
+    <t>Required for non-QC entries</t>
+  </si>
+  <si>
+    <t>Required if Depth entered</t>
+  </si>
+  <si>
+    <t>As needed</t>
+  </si>
+  <si>
+    <t>Leave cells blank if they are not required and they don't need a value.</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Sample Collection Method ID</t>
+  </si>
+  <si>
+    <t>Grab</t>
+  </si>
+  <si>
+    <t>Result Comment</t>
+  </si>
+  <si>
+    <t>Water Quality</t>
+  </si>
+  <si>
+    <t>River was very full</t>
+  </si>
+  <si>
+    <t>defined in WQX by organization</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the Project ID as defined in WQX.  MassWateR will assign a default value of "Water Quality" if nothing is entered.</t>
+  </si>
+  <si>
+    <t>Required for activity type Sample-Routine only</t>
+  </si>
+  <si>
+    <t>Free-form comments about the sample.</t>
+  </si>
+  <si>
+    <t>any note</t>
+  </si>
+  <si>
+    <t>Name of the measured parameter.
+- Note that this can be either the WQX or Simple parameter name.  However, if a parameter is distinguished by Sample Fraction only (i.e. TDP, PON, TDN), then the Simple parameter name must be used here and in all other files (WQX, DQO, etc.).</t>
+  </si>
+  <si>
+    <t>Optional (for analysis) field that can be used to group results using whatever coding system the users wants, such as wet weather or dry weather.
+This field can also be used to record sample IDs for QC samples, such as lab blanks and lab dulicates.</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab", "Pole", and "Basket".</t>
+  </si>
+  <si>
+    <t>Quality Control-Calibration Check</t>
   </si>
   <si>
     <t>Field Msr/Obs
@@ -213,127 +326,9 @@
 Quality Control Sample-Lab Duplicate
 Quality Control Sample-Lab Blank
 Quality Control Sample-Lab Spike
-Quality Control Field Calibration Check</t>
-  </si>
-  <si>
-    <t>user defined</t>
-  </si>
-  <si>
-    <t>Qualification code for samples.  Leave blank for samples that are considered good without question.  Enter "Q" for samples that have been identified as questionable.  Censored samples should not be entered at all.</t>
-  </si>
-  <si>
-    <t>Sampling depth unit of measure.</t>
-  </si>
-  <si>
-    <t>value, BDL, AQL</t>
-  </si>
-  <si>
-    <t>This is used for duplicates, spikes, and calibration checks.  For duplicates, the second value is entered here.  For spikes, the reference target is entered here.  For calibration checks, the target calibration standard is entered here.</t>
-  </si>
-  <si>
-    <t>blank, Q</t>
-  </si>
-  <si>
-    <t>Sampling Time (formatted as time in Excel with correct AM/PM)</t>
-  </si>
-  <si>
-    <t>Numeric measured value.  If the value is below the detection limit, enter "BDL".  If the value is above the quantitation limit, enter "AQL".</t>
-  </si>
-  <si>
-    <t>If the Result Value is BDL or AQL, this column will be checked for the limit value.  If a value is entered here it will be used.  Otherwise, the value in the MDL or UQL column in the DQO Accuracy file will be used.  MassWateR analytical functions will use 1/2 of the MDL and 100% of the UQL.</t>
-  </si>
-  <si>
-    <t>The Results tab must be the first tab in this workbook.</t>
-  </si>
-  <si>
-    <t>Sampling Date (formatted as date in Exel M/D/YYYY)</t>
-  </si>
-  <si>
-    <t>ft, m</t>
-  </si>
-  <si>
-    <t>Surface, Bottom, Midwater, Near Bottom</t>
-  </si>
-  <si>
-    <t>Either Depth or Relative Depth is required.  Relative Depth is a description of the relative depth in the water body, such as "Surface" or "Bottom".  MassWateR analytical functions only evaluate surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
-  </si>
-  <si>
-    <t>Sampling Depth.  MassWateR analytical functions only evaluate surface samples.  It considers all samples &lt; 1 m or &lt; 3.3 ft to be surface samples.  If both Depth and Relative Depth are entered, then Relative Depth should take precedent.</t>
-  </si>
-  <si>
-    <t>Required?</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Either Depth or Relative Depth Required for non-QC entries</t>
-  </si>
-  <si>
-    <t>Required for non-QC entries</t>
-  </si>
-  <si>
-    <t>Required if Depth entered</t>
-  </si>
-  <si>
-    <t>Only for duplicates, spikes, and instrument checks</t>
-  </si>
-  <si>
-    <t>As needed</t>
-  </si>
-  <si>
-    <t>Leave cells blank if they are not required and they don't need a value.</t>
-  </si>
-  <si>
-    <t>Project ID</t>
-  </si>
-  <si>
-    <t>Sample Collection Method ID</t>
-  </si>
-  <si>
-    <t>Grab</t>
-  </si>
-  <si>
-    <t>Result Comment</t>
-  </si>
-  <si>
-    <t>Water Quality</t>
-  </si>
-  <si>
-    <t>River was very full</t>
-  </si>
-  <si>
-    <t>defined in WQX by organization</t>
-  </si>
-  <si>
-    <t>For WQX:  Enter the Project ID as defined in WQX.  MassWateR will assign a default value of "Water Quality" if nothing is entered.</t>
-  </si>
-  <si>
-    <t>Required for activity type Sample-Routine only</t>
-  </si>
-  <si>
-    <t>Free-form comments about the sample.</t>
-  </si>
-  <si>
-    <t>any note</t>
-  </si>
-  <si>
-    <t>Name of the measured parameter.
-- Note that this can be either the WQX or Simple parameter name.  However, if a parameter is distinguished by Sample Fraction only (i.e. TDP, PON, TDN), then the Simple parameter name must be used here and in all other files (WQX, DQO, etc.).</t>
-  </si>
-  <si>
-    <t>Optional (for analysis) field that can be used to group results using whatever coding system the users wants, such as wet weather or dry weather.
-This field can also be used to record sample IDs for QC samples, such as lab blanks and lab dulicates.</t>
-  </si>
-  <si>
-    <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.
-- One exception to this rule is Lab Spikes.  Lab Spikes may be entered for any parameter with a % unit of measure.  "% recovery" is recommended but "%" can also be used.</t>
-  </si>
-  <si>
-    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab", "Pole", and "Basket".</t>
+Quality Control-Meter Lab Duplicate
+Quality Control-Meter Lab Blank
+Quality Control-Calibration Check</t>
   </si>
   <si>
     <r>
@@ -481,7 +476,51 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Quality Control Field Calibration Check</t>
+      <t>Quality Control-Meter Lab Duplicate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - for meter QC lab duplicates.  One value should be entered in the Result Value field and the other value should be entered in the QC Reference Value field.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quality Control-Meter Lab Blank</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - for meter QC lab blanks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quality Control-Calibration Check</t>
     </r>
     <r>
       <rPr>
@@ -494,6 +533,13 @@
       <t xml:space="preserve"> - for post-sampling instrument calibration checks.  The instrument reading should be entered in the Result Value field and the target calibration standard should be entered in the QC Reference Value field.
 Field duplicate results are entered in the QC Reference Value field next the corresponding Field Msr/Obs or Sample-Routine Result Value.</t>
     </r>
+  </si>
+  <si>
+    <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.
+- One exception to this rule is Lab Spikes.  Lab Spikes may be entered with a % unit of measure for any parameter.  "% recovery" is recommended but "%" can also be used.</t>
+  </si>
+  <si>
+    <t>Only for duplicates, spikes, and calibration checks</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1074,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,13 +1139,13 @@
         <v>24</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1137,7 +1183,7 @@
         <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1172,13 +1218,13 @@
         <v>12</v>
       </c>
       <c r="O3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" t="s">
         <v>69</v>
-      </c>
-      <c r="P3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1204,15 +1250,15 @@
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4">
         <v>44451</v>
@@ -1233,7 +1279,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1256,7 +1302,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,34 +1316,34 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="D5" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1305,33 +1351,33 @@
         <v>0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,14 +1385,14 @@
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="18">
         <v>44383</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,14 +1400,14 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="19">
         <v>0.24652777777777801</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1369,14 +1415,14 @@
         <v>4</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="17">
         <v>0.75</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,16 +1430,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1401,16 +1447,16 @@
         <v>25</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1418,16 +1464,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1435,16 +1481,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="17">
         <v>810</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1452,16 +1498,16 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1469,14 +1515,14 @@
         <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="17">
         <v>1500</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1484,14 +1530,14 @@
         <v>20</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" s="17">
         <v>830</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="25" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1499,16 +1545,16 @@
         <v>9</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1516,65 +1562,65 @@
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@8a2f698
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE51E64-D386-4FF2-B8DB-5DD9DE790D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBD60F-CBFB-405D-8835-5C40D5EBF3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>For WQX:  Enter the Project ID as defined in WQX.  MassWateR will assign a default value of "Water Quality" if nothing is entered.</t>
   </si>
   <si>
-    <t>Required for activity type Sample-Routine only</t>
-  </si>
-  <si>
     <t>Free-form comments about the sample.</t>
   </si>
   <si>
@@ -540,6 +537,9 @@
   </si>
   <si>
     <t>Only for duplicates, spikes, and calibration checks</t>
+  </si>
+  <si>
+    <t>Required for activity types Sample-Routine and Quality Control Sample-Field Blank</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4">
         <v>44451</v>
@@ -1302,7 +1302,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,13 +1368,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>57</v>
@@ -1464,7 +1464,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
@@ -1498,7 +1498,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
@@ -1579,7 +1579,7 @@
         <v>65</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>66</v>
@@ -1588,7 +1588,7 @@
         <v>70</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1613,10 +1613,10 @@
         <v>67</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">

</xml_diff>

<commit_message>
Built site for MassWateR: 2.0.0@a9cf368
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBD60F-CBFB-405D-8835-5C40D5EBF3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69C043D-D8C9-4955-8F56-EE0F135187CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>Sample Collection Method ID</t>
   </si>
   <si>
-    <t>Grab</t>
-  </si>
-  <si>
     <t>Result Comment</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
   <si>
     <t>Optional (for analysis) field that can be used to group results using whatever coding system the users wants, such as wet weather or dry weather.
 This field can also be used to record sample IDs for QC samples, such as lab blanks and lab dulicates.</t>
-  </si>
-  <si>
-    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab", "Pole", and "Basket".</t>
   </si>
   <si>
     <t>Quality Control-Calibration Check</t>
@@ -540,6 +534,12 @@
   </si>
   <si>
     <t>Required for activity types Sample-Routine and Quality Control Sample-Field Blank</t>
+  </si>
+  <si>
+    <t>Grab-MassWateR</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab-MassWateR" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab-MassWateR", "Pole-MassWateR", and "Basket-MassWateR".</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1074,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1145,7 @@
         <v>64</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1218,13 +1218,13 @@
         <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="P3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" t="s">
         <v>68</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1253,12 +1253,12 @@
         <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4">
         <v>44451</v>
@@ -1279,7 +1279,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1302,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,13 +1368,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>57</v>
@@ -1464,7 +1464,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
@@ -1498,7 +1498,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
@@ -1579,16 +1579,16 @@
         <v>65</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1596,13 +1596,13 @@
         <v>64</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>57</v>
@@ -1610,13 +1610,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>73</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">

</xml_diff>

<commit_message>
Built site for MassWateR: 2.0.2.9000@04ce74b
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69C043D-D8C9-4955-8F56-EE0F135187CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A57075-EBC7-4D53-B5FE-E18A96337DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="Values" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$N$1</definedName>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="191">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -541,6 +542,330 @@
   <si>
     <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab-MassWateR" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab-MassWateR", "Pole-MassWateR", and "Basket-MassWateR".</t>
   </si>
+  <si>
+    <t>3-1-17_345367</t>
+  </si>
+  <si>
+    <t>Free-form field for capturing a locally defined unique identifier for each record.  Only needed if your local system has a record identifier that you want to keep track of in WQX.</t>
+  </si>
+  <si>
+    <t>Local Record ID</t>
+  </si>
+  <si>
+    <t>Quality Control Sample-Field Blank</t>
+  </si>
+  <si>
+    <t>Quality Control Sample-Lab Blank</t>
+  </si>
+  <si>
+    <t>Quality Control Sample-Lab Spike</t>
+  </si>
+  <si>
+    <t>Quality Control-Meter Lab Duplicate</t>
+  </si>
+  <si>
+    <t>Quality Control-Meter Lab Blank</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Midwater</t>
+  </si>
+  <si>
+    <t>Near Bottom</t>
+  </si>
+  <si>
+    <t>Water Temp</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Ortho P</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>TDP</t>
+  </si>
+  <si>
+    <t>Nitrite</t>
+  </si>
+  <si>
+    <t>Nitrate + Nitrite</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TKN</t>
+  </si>
+  <si>
+    <t>PON</t>
+  </si>
+  <si>
+    <t>TDN</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Ammonium</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>Silicate</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Turbidity</t>
+  </si>
+  <si>
+    <t>Secchi Depth</t>
+  </si>
+  <si>
+    <t>Chl a</t>
+  </si>
+  <si>
+    <t>Chl a (probe)</t>
+  </si>
+  <si>
+    <t>Pheophytin</t>
+  </si>
+  <si>
+    <t>Enterococcus</t>
+  </si>
+  <si>
+    <t>Fecal Coliform</t>
+  </si>
+  <si>
+    <t>Surfactants</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (probe)</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (lab)</t>
+  </si>
+  <si>
+    <t>Microcystins</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Gage</t>
+  </si>
+  <si>
+    <t>Air Temp</t>
+  </si>
+  <si>
+    <t>Temperature, water</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen (DO)</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen saturation</t>
+  </si>
+  <si>
+    <t>Specific conductance</t>
+  </si>
+  <si>
+    <t>Total Phosphorus, mixed forms</t>
+  </si>
+  <si>
+    <t>Orthophosphate</t>
+  </si>
+  <si>
+    <t>Phosphorus, Particulate Organic</t>
+  </si>
+  <si>
+    <t>Total Nitrogen, mixed forms</t>
+  </si>
+  <si>
+    <t>Total Kjeldahl nitrogen</t>
+  </si>
+  <si>
+    <t>Particulate organic carbon</t>
+  </si>
+  <si>
+    <t>Total suspended solids</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>Depth, Secchi disk depth</t>
+  </si>
+  <si>
+    <t>Chlorophyll a</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (probe)</t>
+  </si>
+  <si>
+    <t>Pheophytin a</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (probe) concentration, Cyanobacteria (bluegreen)</t>
+  </si>
+  <si>
+    <t>Algae, blue-green (phylum cyanophyta) density</t>
+  </si>
+  <si>
+    <t>Height, gage</t>
+  </si>
+  <si>
+    <t>Temperature, air</t>
+  </si>
+  <si>
+    <t>ug/l</t>
+  </si>
+  <si>
+    <t>umol/l</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>deg C</t>
+  </si>
+  <si>
+    <t>deg F</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>s.u.</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>PSS</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>ppt</t>
+  </si>
+  <si>
+    <t>ppth</t>
+  </si>
+  <si>
+    <t>mS/cm</t>
+  </si>
+  <si>
+    <t>S/m</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>MPN/100ml</t>
+  </si>
+  <si>
+    <t>#/100ml</t>
+  </si>
+  <si>
+    <t>cfs</t>
+  </si>
+  <si>
+    <t>cfm</t>
+  </si>
+  <si>
+    <t>mgd</t>
+  </si>
+  <si>
+    <t>l/min</t>
+  </si>
+  <si>
+    <t>l/sec</t>
+  </si>
+  <si>
+    <t>FNU</t>
+  </si>
+  <si>
+    <t>JTU</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>FAU</t>
+  </si>
+  <si>
+    <t>FBU</t>
+  </si>
+  <si>
+    <t>FNMU</t>
+  </si>
+  <si>
+    <t>FNRU</t>
+  </si>
+  <si>
+    <t>NTMU</t>
+  </si>
+  <si>
+    <t>NTRU</t>
+  </si>
+  <si>
+    <t>FTU</t>
+  </si>
+  <si>
+    <t>Pole-MassWateR</t>
+  </si>
+  <si>
+    <t>Basket-MassWateR</t>
+  </si>
+  <si>
+    <t>Template updated 4/7/23</t>
+  </si>
 </sst>
 </file>
 
@@ -549,7 +874,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,8 +919,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +955,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +1020,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -753,6 +1091,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,13 +1410,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,10 +1434,11 @@
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1145,10 +1488,13 @@
         <v>64</v>
       </c>
       <c r="Q1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1186,7 +1532,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1215,7 +1561,7 @@
         <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="O3" t="s">
         <v>81</v>
@@ -1223,11 +1569,11 @@
       <c r="P3" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1256,7 +1602,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -1291,12 +1637,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{32BB1E41-7B7C-4040-A5BC-F0F361CEF4ED}">
+          <x14:formula1>
+            <xm:f>Values!$A$2:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A1C28841-16D0-4E3A-A64E-6BE7E75B23E2}">
+          <x14:formula1>
+            <xm:f>Values!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{3D252FD9-0DEB-46E0-8BC7-67012DA2692C}">
+          <x14:formula1>
+            <xm:f>Values!$C$2:$C$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28137517-E795-4631-83B1-DD4616788B35}">
+          <x14:formula1>
+            <xm:f>Values!$D$2:$D$87</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DAA8724F-43C6-4451-A490-9132A9A6EAA5}">
+          <x14:formula1>
+            <xm:f>Values!$E$2:$E$41</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D8A1554-0B5F-4912-9C2C-B7455F484847}">
+          <x14:formula1>
+            <xm:f>Values!$F$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{A40CB64D-C991-409E-9DB0-D13C47A34E8E}">
+          <x14:formula1>
+            <xm:f>Values!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78C6628-51AC-4A46-96D9-F2FA0EFA1B4C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -1318,6 +1712,9 @@
       <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
+      <c r="C1" s="27" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -1608,18 +2005,35 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B23" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="25" t="s">
+      <c r="D23" s="17"/>
+      <c r="E23" s="25" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1627,4 +2041,666 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2711FA19-F675-4631-8E5F-6D018E88F2B7}">
+  <dimension ref="A1:L87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D87">
+    <sortCondition ref="D2:D87"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Built site for MassWateR: 2.0.2.9000@5369134
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A57075-EBC7-4D53-B5FE-E18A96337DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69C043D-D8C9-4955-8F56-EE0F135187CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
-    <sheet name="Values" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$N$1</definedName>
@@ -80,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -542,330 +541,6 @@
   <si>
     <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab-MassWateR" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab-MassWateR", "Pole-MassWateR", and "Basket-MassWateR".</t>
   </si>
-  <si>
-    <t>3-1-17_345367</t>
-  </si>
-  <si>
-    <t>Free-form field for capturing a locally defined unique identifier for each record.  Only needed if your local system has a record identifier that you want to keep track of in WQX.</t>
-  </si>
-  <si>
-    <t>Local Record ID</t>
-  </si>
-  <si>
-    <t>Quality Control Sample-Field Blank</t>
-  </si>
-  <si>
-    <t>Quality Control Sample-Lab Blank</t>
-  </si>
-  <si>
-    <t>Quality Control Sample-Lab Spike</t>
-  </si>
-  <si>
-    <t>Quality Control-Meter Lab Duplicate</t>
-  </si>
-  <si>
-    <t>Quality Control-Meter Lab Blank</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Bottom</t>
-  </si>
-  <si>
-    <t>Midwater</t>
-  </si>
-  <si>
-    <t>Near Bottom</t>
-  </si>
-  <si>
-    <t>Water Temp</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>DO</t>
-  </si>
-  <si>
-    <t>Conductivity</t>
-  </si>
-  <si>
-    <t>Salinity</t>
-  </si>
-  <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>Ortho P</t>
-  </si>
-  <si>
-    <t>POP</t>
-  </si>
-  <si>
-    <t>TDP</t>
-  </si>
-  <si>
-    <t>Nitrite</t>
-  </si>
-  <si>
-    <t>Nitrate + Nitrite</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>TKN</t>
-  </si>
-  <si>
-    <t>PON</t>
-  </si>
-  <si>
-    <t>TDN</t>
-  </si>
-  <si>
-    <t>Ammonia</t>
-  </si>
-  <si>
-    <t>Ammonium</t>
-  </si>
-  <si>
-    <t>POC</t>
-  </si>
-  <si>
-    <t>Silicate</t>
-  </si>
-  <si>
-    <t>Chloride</t>
-  </si>
-  <si>
-    <t>Sulfate</t>
-  </si>
-  <si>
-    <t>TDS</t>
-  </si>
-  <si>
-    <t>Turbidity</t>
-  </si>
-  <si>
-    <t>Secchi Depth</t>
-  </si>
-  <si>
-    <t>Chl a</t>
-  </si>
-  <si>
-    <t>Chl a (probe)</t>
-  </si>
-  <si>
-    <t>Pheophytin</t>
-  </si>
-  <si>
-    <t>Enterococcus</t>
-  </si>
-  <si>
-    <t>Fecal Coliform</t>
-  </si>
-  <si>
-    <t>Surfactants</t>
-  </si>
-  <si>
-    <t>Cyanobacteria (probe)</t>
-  </si>
-  <si>
-    <t>Cyanobacteria (lab)</t>
-  </si>
-  <si>
-    <t>Microcystins</t>
-  </si>
-  <si>
-    <t>Metals</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Depth</t>
-  </si>
-  <si>
-    <t>Gage</t>
-  </si>
-  <si>
-    <t>Air Temp</t>
-  </si>
-  <si>
-    <t>Temperature, water</t>
-  </si>
-  <si>
-    <t>Dissolved oxygen (DO)</t>
-  </si>
-  <si>
-    <t>Dissolved oxygen saturation</t>
-  </si>
-  <si>
-    <t>Specific conductance</t>
-  </si>
-  <si>
-    <t>Total Phosphorus, mixed forms</t>
-  </si>
-  <si>
-    <t>Orthophosphate</t>
-  </si>
-  <si>
-    <t>Phosphorus, Particulate Organic</t>
-  </si>
-  <si>
-    <t>Total Nitrogen, mixed forms</t>
-  </si>
-  <si>
-    <t>Total Kjeldahl nitrogen</t>
-  </si>
-  <si>
-    <t>Particulate organic carbon</t>
-  </si>
-  <si>
-    <t>Total suspended solids</t>
-  </si>
-  <si>
-    <t>Total dissolved solids</t>
-  </si>
-  <si>
-    <t>Depth, Secchi disk depth</t>
-  </si>
-  <si>
-    <t>Chlorophyll a</t>
-  </si>
-  <si>
-    <t>Chlorophyll a (probe)</t>
-  </si>
-  <si>
-    <t>Pheophytin a</t>
-  </si>
-  <si>
-    <t>Escherichia coli</t>
-  </si>
-  <si>
-    <t>Chlorophyll a (probe) concentration, Cyanobacteria (bluegreen)</t>
-  </si>
-  <si>
-    <t>Algae, blue-green (phylum cyanophyta) density</t>
-  </si>
-  <si>
-    <t>Height, gage</t>
-  </si>
-  <si>
-    <t>Temperature, air</t>
-  </si>
-  <si>
-    <t>ug/l</t>
-  </si>
-  <si>
-    <t>umol/l</t>
-  </si>
-  <si>
-    <t>ppm</t>
-  </si>
-  <si>
-    <t>deg C</t>
-  </si>
-  <si>
-    <t>deg F</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>s.u.</t>
-  </si>
-  <si>
-    <t>PSU</t>
-  </si>
-  <si>
-    <t>PSS</t>
-  </si>
-  <si>
-    <t>g/kg</t>
-  </si>
-  <si>
-    <t>ppt</t>
-  </si>
-  <si>
-    <t>ppth</t>
-  </si>
-  <si>
-    <t>mS/cm</t>
-  </si>
-  <si>
-    <t>S/m</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>MPN/100ml</t>
-  </si>
-  <si>
-    <t>#/100ml</t>
-  </si>
-  <si>
-    <t>cfs</t>
-  </si>
-  <si>
-    <t>cfm</t>
-  </si>
-  <si>
-    <t>mgd</t>
-  </si>
-  <si>
-    <t>l/min</t>
-  </si>
-  <si>
-    <t>l/sec</t>
-  </si>
-  <si>
-    <t>FNU</t>
-  </si>
-  <si>
-    <t>JTU</t>
-  </si>
-  <si>
-    <t>NTU</t>
-  </si>
-  <si>
-    <t>AU</t>
-  </si>
-  <si>
-    <t>BU</t>
-  </si>
-  <si>
-    <t>FAU</t>
-  </si>
-  <si>
-    <t>FBU</t>
-  </si>
-  <si>
-    <t>FNMU</t>
-  </si>
-  <si>
-    <t>FNRU</t>
-  </si>
-  <si>
-    <t>NTMU</t>
-  </si>
-  <si>
-    <t>NTRU</t>
-  </si>
-  <si>
-    <t>FTU</t>
-  </si>
-  <si>
-    <t>Pole-MassWateR</t>
-  </si>
-  <si>
-    <t>Basket-MassWateR</t>
-  </si>
-  <si>
-    <t>Template updated 4/7/23</t>
-  </si>
 </sst>
 </file>
 
@@ -874,7 +549,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -919,15 +594,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,12 +623,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1091,10 +753,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1410,13 +1068,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,11 +1092,10 @@
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1488,13 +1145,10 @@
         <v>64</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="R1" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1532,7 +1186,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1561,7 +1215,7 @@
         <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
         <v>81</v>
@@ -1569,11 +1223,11 @@
       <c r="P3" t="s">
         <v>67</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Q3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1256,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -1637,60 +1291,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{32BB1E41-7B7C-4040-A5BC-F0F361CEF4ED}">
-          <x14:formula1>
-            <xm:f>Values!$A$2:$A$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A1C28841-16D0-4E3A-A64E-6BE7E75B23E2}">
-          <x14:formula1>
-            <xm:f>Values!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{3D252FD9-0DEB-46E0-8BC7-67012DA2692C}">
-          <x14:formula1>
-            <xm:f>Values!$C$2:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28137517-E795-4631-83B1-DD4616788B35}">
-          <x14:formula1>
-            <xm:f>Values!$D$2:$D$87</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DAA8724F-43C6-4451-A490-9132A9A6EAA5}">
-          <x14:formula1>
-            <xm:f>Values!$E$2:$E$41</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D8A1554-0B5F-4912-9C2C-B7455F484847}">
-          <x14:formula1>
-            <xm:f>Values!$F$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{A40CB64D-C991-409E-9DB0-D13C47A34E8E}">
-          <x14:formula1>
-            <xm:f>Values!$G$2:$G$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2:O1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78C6628-51AC-4A46-96D9-F2FA0EFA1B4C}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -1712,9 +1318,6 @@
       <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -2005,35 +1608,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>41</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D22" s="17"/>
       <c r="E22" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="25" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2041,666 +1627,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2711FA19-F675-4631-8E5F-6D018E88F2B7}">
-  <dimension ref="A1:L87"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" t="s">
-        <v>179</v>
-      </c>
-      <c r="G4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>145</v>
-      </c>
-      <c r="E21" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E29" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>152</v>
-      </c>
-      <c r="E35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>128</v>
-      </c>
-      <c r="E36" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>128</v>
-      </c>
-      <c r="E37" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D87">
-    <sortCondition ref="D2:D87"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Built site for MassWateR: 2.1.0@da49601
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08D7B72-B552-4985-90AF-3CAAF37FE061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2A3B6C-510B-4645-B614-6E16FA3EE76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="192">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -867,7 +867,7 @@
     <t>% recovery</t>
   </si>
   <si>
-    <t>Template updated 5/4/23</t>
+    <t>Template updated 6/29/23</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1419,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,12 +1661,6 @@
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28137517-E795-4631-83B1-DD4616788B35}">
-          <x14:formula1>
-            <xm:f>Values!$D$2:$D$87</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D8A1554-0B5F-4912-9C2C-B7455F484847}">
           <x14:formula1>
             <xm:f>Values!$F$2</xm:f>
@@ -1684,6 +1678,12 @@
             <xm:f>Values!$E$2:$E$42</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28137517-E795-4631-83B1-DD4616788B35}">
+          <x14:formula1>
+            <xm:f>Values!$D$2:$D$65</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2048,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2711FA19-F675-4631-8E5F-6D018E88F2B7}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2160,7 @@
         <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
         <v>179</v>
@@ -2171,7 +2171,7 @@
         <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E6" t="s">
         <v>180</v>
@@ -2182,7 +2182,7 @@
         <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
         <v>172</v>
@@ -2193,7 +2193,7 @@
         <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
         <v>171</v>
@@ -2204,7 +2204,7 @@
         <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -2215,7 +2215,7 @@
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
         <v>168</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="E11" t="s">
         <v>157</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
         <v>158</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
         <v>181</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
         <v>182</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="E15" t="s">
         <v>183</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
         <v>184</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
         <v>176</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
         <v>187</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
         <v>163</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
         <v>177</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
         <v>174</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="E23" t="s">
         <v>175</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="E24" t="s">
         <v>91</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>27</v>
+        <v>129</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="E26" t="s">
         <v>173</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
         <v>169</v>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
         <v>166</v>
@@ -2367,7 +2367,7 @@
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="E29" t="s">
         <v>159</v>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
         <v>185</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="E31" t="s">
         <v>186</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="E32" t="s">
         <v>178</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
         <v>156</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E34" t="s">
         <v>164</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
         <v>165</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
         <v>162</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E37" t="s">
         <v>161</v>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="E38" t="s">
         <v>160</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="E39" t="s">
         <v>167</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="E40" t="s">
         <v>154</v>
@@ -2463,7 +2463,7 @@
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
         <v>155</v>
@@ -2471,7 +2471,7 @@
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
         <v>31</v>
@@ -2479,232 +2479,122 @@
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D87">
-    <sortCondition ref="D2:D87"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D65">
+    <sortCondition ref="D2:D65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Built site for MassWateR: 2.1.1@5258357
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2A3B6C-510B-4645-B614-6E16FA3EE76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E938E-1C2A-4248-B6A3-B6B6105ADE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -527,347 +527,347 @@
     </r>
   </si>
   <si>
+    <t>Only for duplicates, spikes, and calibration checks</t>
+  </si>
+  <si>
+    <t>Required for activity types Sample-Routine and Quality Control Sample-Field Blank</t>
+  </si>
+  <si>
+    <t>Grab-MassWateR</t>
+  </si>
+  <si>
+    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab-MassWateR" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab-MassWateR", "Pole-MassWateR", and "Basket-MassWateR".</t>
+  </si>
+  <si>
+    <t>3-1-17_345367</t>
+  </si>
+  <si>
+    <t>Free-form field for capturing a locally defined unique identifier for each record.  Only needed if your local system has a record identifier that you want to keep track of in WQX.</t>
+  </si>
+  <si>
+    <t>Local Record ID</t>
+  </si>
+  <si>
+    <t>Quality Control Sample-Field Blank</t>
+  </si>
+  <si>
+    <t>Quality Control Sample-Lab Blank</t>
+  </si>
+  <si>
+    <t>Quality Control Sample-Lab Spike</t>
+  </si>
+  <si>
+    <t>Quality Control-Meter Lab Duplicate</t>
+  </si>
+  <si>
+    <t>Quality Control-Meter Lab Blank</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Midwater</t>
+  </si>
+  <si>
+    <t>Near Bottom</t>
+  </si>
+  <si>
+    <t>Water Temp</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Ortho P</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>TDP</t>
+  </si>
+  <si>
+    <t>Nitrite</t>
+  </si>
+  <si>
+    <t>Nitrate + Nitrite</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TKN</t>
+  </si>
+  <si>
+    <t>PON</t>
+  </si>
+  <si>
+    <t>TDN</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Ammonium</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>Silicate</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Turbidity</t>
+  </si>
+  <si>
+    <t>Secchi Depth</t>
+  </si>
+  <si>
+    <t>Chl a</t>
+  </si>
+  <si>
+    <t>Chl a (probe)</t>
+  </si>
+  <si>
+    <t>Pheophytin</t>
+  </si>
+  <si>
+    <t>Enterococcus</t>
+  </si>
+  <si>
+    <t>Fecal Coliform</t>
+  </si>
+  <si>
+    <t>Surfactants</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (probe)</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (lab)</t>
+  </si>
+  <si>
+    <t>Microcystins</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Gage</t>
+  </si>
+  <si>
+    <t>Air Temp</t>
+  </si>
+  <si>
+    <t>Temperature, water</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen (DO)</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen saturation</t>
+  </si>
+  <si>
+    <t>Specific conductance</t>
+  </si>
+  <si>
+    <t>Total Phosphorus, mixed forms</t>
+  </si>
+  <si>
+    <t>Orthophosphate</t>
+  </si>
+  <si>
+    <t>Phosphorus, Particulate Organic</t>
+  </si>
+  <si>
+    <t>Total Nitrogen, mixed forms</t>
+  </si>
+  <si>
+    <t>Total Kjeldahl nitrogen</t>
+  </si>
+  <si>
+    <t>Particulate organic carbon</t>
+  </si>
+  <si>
+    <t>Total suspended solids</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>Depth, Secchi disk depth</t>
+  </si>
+  <si>
+    <t>Chlorophyll a</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (probe)</t>
+  </si>
+  <si>
+    <t>Pheophytin a</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (probe) concentration, Cyanobacteria (bluegreen)</t>
+  </si>
+  <si>
+    <t>Algae, blue-green (phylum cyanophyta) density</t>
+  </si>
+  <si>
+    <t>Height, gage</t>
+  </si>
+  <si>
+    <t>Temperature, air</t>
+  </si>
+  <si>
+    <t>ug/l</t>
+  </si>
+  <si>
+    <t>umol/l</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>deg C</t>
+  </si>
+  <si>
+    <t>deg F</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>s.u.</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>PSS</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>ppt</t>
+  </si>
+  <si>
+    <t>ppth</t>
+  </si>
+  <si>
+    <t>mS/cm</t>
+  </si>
+  <si>
+    <t>S/m</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>MPN/100ml</t>
+  </si>
+  <si>
+    <t>#/100ml</t>
+  </si>
+  <si>
+    <t>cfs</t>
+  </si>
+  <si>
+    <t>cfm</t>
+  </si>
+  <si>
+    <t>mgd</t>
+  </si>
+  <si>
+    <t>l/min</t>
+  </si>
+  <si>
+    <t>l/sec</t>
+  </si>
+  <si>
+    <t>FNU</t>
+  </si>
+  <si>
+    <t>JTU</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>FAU</t>
+  </si>
+  <si>
+    <t>FBU</t>
+  </si>
+  <si>
+    <t>FNMU</t>
+  </si>
+  <si>
+    <t>FNRU</t>
+  </si>
+  <si>
+    <t>NTMU</t>
+  </si>
+  <si>
+    <t>NTRU</t>
+  </si>
+  <si>
+    <t>FTU</t>
+  </si>
+  <si>
+    <t>Pole-MassWateR</t>
+  </si>
+  <si>
+    <t>Basket-MassWateR</t>
+  </si>
+  <si>
+    <t>% recovery</t>
+  </si>
+  <si>
     <t>Result unit of measure.  Only the units of measure listed in the parameter list are allowed.  The unit of measure used for each parameter must be consistent for the whole file.
-- One exception to this rule is Lab Spikes.  Lab Spikes may be entered with a % unit of measure for any parameter.  "% recovery" is recommended but "%" can also be used.</t>
-  </si>
-  <si>
-    <t>Only for duplicates, spikes, and calibration checks</t>
-  </si>
-  <si>
-    <t>Required for activity types Sample-Routine and Quality Control Sample-Field Blank</t>
-  </si>
-  <si>
-    <t>Grab-MassWateR</t>
-  </si>
-  <si>
-    <t>For WQX:  Enter the method ID used for this sample collection.  Not applicable for field measurement/observations.  Method IDs are defined in WQX by organization.  MassWateR will assign a default value of "Grab-MassWateR" if nothing is entered, but this requires a Method Context of "MassWateR" in the WQXMeta file.  Standard method IDs that can be used by any organization under the MassWateR context are "Grab-MassWateR", "Pole-MassWateR", and "Basket-MassWateR".</t>
-  </si>
-  <si>
-    <t>3-1-17_345367</t>
-  </si>
-  <si>
-    <t>Free-form field for capturing a locally defined unique identifier for each record.  Only needed if your local system has a record identifier that you want to keep track of in WQX.</t>
-  </si>
-  <si>
-    <t>Local Record ID</t>
-  </si>
-  <si>
-    <t>Quality Control Sample-Field Blank</t>
-  </si>
-  <si>
-    <t>Quality Control Sample-Lab Blank</t>
-  </si>
-  <si>
-    <t>Quality Control Sample-Lab Spike</t>
-  </si>
-  <si>
-    <t>Quality Control-Meter Lab Duplicate</t>
-  </si>
-  <si>
-    <t>Quality Control-Meter Lab Blank</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Bottom</t>
-  </si>
-  <si>
-    <t>Midwater</t>
-  </si>
-  <si>
-    <t>Near Bottom</t>
-  </si>
-  <si>
-    <t>Water Temp</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>DO</t>
-  </si>
-  <si>
-    <t>Conductivity</t>
-  </si>
-  <si>
-    <t>Salinity</t>
-  </si>
-  <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>Ortho P</t>
-  </si>
-  <si>
-    <t>POP</t>
-  </si>
-  <si>
-    <t>TDP</t>
-  </si>
-  <si>
-    <t>Nitrite</t>
-  </si>
-  <si>
-    <t>Nitrate + Nitrite</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>TKN</t>
-  </si>
-  <si>
-    <t>PON</t>
-  </si>
-  <si>
-    <t>TDN</t>
-  </si>
-  <si>
-    <t>Ammonia</t>
-  </si>
-  <si>
-    <t>Ammonium</t>
-  </si>
-  <si>
-    <t>POC</t>
-  </si>
-  <si>
-    <t>Silicate</t>
-  </si>
-  <si>
-    <t>Chloride</t>
-  </si>
-  <si>
-    <t>Sulfate</t>
-  </si>
-  <si>
-    <t>TDS</t>
-  </si>
-  <si>
-    <t>Turbidity</t>
-  </si>
-  <si>
-    <t>Secchi Depth</t>
-  </si>
-  <si>
-    <t>Chl a</t>
-  </si>
-  <si>
-    <t>Chl a (probe)</t>
-  </si>
-  <si>
-    <t>Pheophytin</t>
-  </si>
-  <si>
-    <t>Enterococcus</t>
-  </si>
-  <si>
-    <t>Fecal Coliform</t>
-  </si>
-  <si>
-    <t>Surfactants</t>
-  </si>
-  <si>
-    <t>Cyanobacteria (probe)</t>
-  </si>
-  <si>
-    <t>Cyanobacteria (lab)</t>
-  </si>
-  <si>
-    <t>Microcystins</t>
-  </si>
-  <si>
-    <t>Metals</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Depth</t>
-  </si>
-  <si>
-    <t>Gage</t>
-  </si>
-  <si>
-    <t>Air Temp</t>
-  </si>
-  <si>
-    <t>Temperature, water</t>
-  </si>
-  <si>
-    <t>Dissolved oxygen (DO)</t>
-  </si>
-  <si>
-    <t>Dissolved oxygen saturation</t>
-  </si>
-  <si>
-    <t>Specific conductance</t>
-  </si>
-  <si>
-    <t>Total Phosphorus, mixed forms</t>
-  </si>
-  <si>
-    <t>Orthophosphate</t>
-  </si>
-  <si>
-    <t>Phosphorus, Particulate Organic</t>
-  </si>
-  <si>
-    <t>Total Nitrogen, mixed forms</t>
-  </si>
-  <si>
-    <t>Total Kjeldahl nitrogen</t>
-  </si>
-  <si>
-    <t>Particulate organic carbon</t>
-  </si>
-  <si>
-    <t>Total suspended solids</t>
-  </si>
-  <si>
-    <t>Total dissolved solids</t>
-  </si>
-  <si>
-    <t>Depth, Secchi disk depth</t>
-  </si>
-  <si>
-    <t>Chlorophyll a</t>
-  </si>
-  <si>
-    <t>Chlorophyll a (probe)</t>
-  </si>
-  <si>
-    <t>Pheophytin a</t>
-  </si>
-  <si>
-    <t>Escherichia coli</t>
-  </si>
-  <si>
-    <t>Chlorophyll a (probe) concentration, Cyanobacteria (bluegreen)</t>
-  </si>
-  <si>
-    <t>Algae, blue-green (phylum cyanophyta) density</t>
-  </si>
-  <si>
-    <t>Height, gage</t>
-  </si>
-  <si>
-    <t>Temperature, air</t>
-  </si>
-  <si>
-    <t>ug/l</t>
-  </si>
-  <si>
-    <t>umol/l</t>
-  </si>
-  <si>
-    <t>ppm</t>
-  </si>
-  <si>
-    <t>deg C</t>
-  </si>
-  <si>
-    <t>deg F</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>s.u.</t>
-  </si>
-  <si>
-    <t>PSU</t>
-  </si>
-  <si>
-    <t>PSS</t>
-  </si>
-  <si>
-    <t>g/kg</t>
-  </si>
-  <si>
-    <t>ppt</t>
-  </si>
-  <si>
-    <t>ppth</t>
-  </si>
-  <si>
-    <t>mS/cm</t>
-  </si>
-  <si>
-    <t>S/m</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>MPN/100ml</t>
-  </si>
-  <si>
-    <t>#/100ml</t>
-  </si>
-  <si>
-    <t>cfs</t>
-  </si>
-  <si>
-    <t>cfm</t>
-  </si>
-  <si>
-    <t>mgd</t>
-  </si>
-  <si>
-    <t>l/min</t>
-  </si>
-  <si>
-    <t>l/sec</t>
-  </si>
-  <si>
-    <t>FNU</t>
-  </si>
-  <si>
-    <t>JTU</t>
-  </si>
-  <si>
-    <t>NTU</t>
-  </si>
-  <si>
-    <t>AU</t>
-  </si>
-  <si>
-    <t>BU</t>
-  </si>
-  <si>
-    <t>FAU</t>
-  </si>
-  <si>
-    <t>FBU</t>
-  </si>
-  <si>
-    <t>FNMU</t>
-  </si>
-  <si>
-    <t>FNRU</t>
-  </si>
-  <si>
-    <t>NTMU</t>
-  </si>
-  <si>
-    <t>NTRU</t>
-  </si>
-  <si>
-    <t>FTU</t>
-  </si>
-  <si>
-    <t>Pole-MassWateR</t>
-  </si>
-  <si>
-    <t>Basket-MassWateR</t>
-  </si>
-  <si>
-    <t>% recovery</t>
-  </si>
-  <si>
-    <t>Template updated 6/29/23</t>
+- One exception to this rule is Lab Spikes.  Lab Spikes may be entered with a % unit of measure for any parameter.  "% recovery" is recommended but "%" can also be used.  Note that if % or % recovery are used, then the Lab Spike DQO must also be defined as a %.</t>
+  </si>
+  <si>
+    <t>Template updated 9/7/23</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1491,7 @@
         <v>64</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>66</v>
@@ -1567,7 +1567,7 @@
         <v>16</v>
       </c>
       <c r="O3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P3" t="s">
         <v>67</v>
@@ -1893,12 +1893,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1979,16 +1979,16 @@
         <v>65</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>69</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2010,13 +2010,13 @@
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>41</v>
@@ -2103,16 +2103,16 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2120,36 +2120,36 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
         <v>91</v>
       </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2157,54 +2157,54 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -2215,71 +2215,71 @@
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -2287,10 +2287,10 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
@@ -2298,7 +2298,7 @@
         <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
@@ -2306,36 +2306,36 @@
         <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
@@ -2343,34 +2343,34 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.25">
@@ -2378,100 +2378,100 @@
         <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E42" t="s">
         <v>31</v>
@@ -2479,17 +2479,17 @@
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.25">
@@ -2499,82 +2499,82 @@
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.25">
@@ -2584,12 +2584,12 @@
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Built site for MassWateR: 2.1.4@692d4a8
</commit_message>
<xml_diff>
--- a/MassWateR_Results_Template.xlsx
+++ b/MassWateR_Results_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d8cbaaa4eaa566d/Documents/1 ACASAK/MassWateR/Design/Templates for users/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E938E-1C2A-4248-B6A3-B6B6105ADE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D99E938E-1C2A-4248-B6A3-B6B6105ADE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C2AECD5-0AD5-45BC-87F6-69F5D8D88A2C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="194">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>Numeric measured value.  If the value is below the detection limit, enter "BDL".  If the value is above the quantitation limit, enter "AQL".</t>
-  </si>
-  <si>
-    <t>If the Result Value is BDL or AQL, this column will be checked for the limit value.  If a value is entered here it will be used.  Otherwise, the value in the MDL or UQL column in the DQO Accuracy file will be used.  MassWateR analytical functions will use 1/2 of the MDL and 100% of the UQL.</t>
   </si>
   <si>
     <t>The Results tab must be the first tab in this workbook.</t>
@@ -867,7 +864,18 @@
 - One exception to this rule is Lab Spikes.  Lab Spikes may be entered with a % unit of measure for any parameter.  "% recovery" is recommended but "%" can also be used.  Note that if % or % recovery are used, then the Lab Spike DQO must also be defined as a %.</t>
   </si>
   <si>
-    <t>Template updated 9/7/23</t>
+    <t>numeric values only</t>
+  </si>
+  <si>
+    <t>Template updated 2/1/24</t>
+  </si>
+  <si>
+    <t>If the Result Value or QC Reference Value is BDL or AQL, this column will be checked for the minimum or upper limit value.  If a value is entered here it will be used.  Otherwise, the value in the MDL or UQL column in the DQO Accuracy file will be used.  This field should only be used to override the values in the DQO Accuracy file.  MassWateR analytical functions will convert BDL to 1/2 of the minimum limit and AQL to 100% of the upper limit.</t>
+  </si>
+  <si>
+    <t>0.01
+or
+1500</t>
   </si>
 </sst>
 </file>
@@ -1116,9 +1124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1156,7 +1164,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1262,7 +1270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1404,7 +1412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1485,16 +1493,16 @@
         <v>24</v>
       </c>
       <c r="O1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1532,7 +1540,7 @@
         <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1567,13 +1575,13 @@
         <v>16</v>
       </c>
       <c r="O3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P3" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" t="s">
         <v>67</v>
-      </c>
-      <c r="R3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1602,12 +1610,12 @@
         <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4">
         <v>44451</v>
@@ -1628,7 +1636,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1696,10 +1704,10 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,12 +1729,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1743,7 +1751,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1760,7 +1768,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="300" x14ac:dyDescent="0.25">
@@ -1768,16 +1776,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,14 +1793,14 @@
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="18">
         <v>44383</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,7 +1815,7 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1815,14 +1823,14 @@
         <v>4</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="17">
         <v>0.75</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,10 +1844,10 @@
         <v>11</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1847,16 +1855,16 @@
         <v>25</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1864,7 +1872,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>29</v>
@@ -1873,7 +1881,7 @@
         <v>40</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1890,7 +1898,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1898,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>32</v>
@@ -1907,22 +1915,24 @@
         <v>40</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="17">
-        <v>1500</v>
-      </c>
-      <c r="D16" s="17"/>
+        <v>192</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>190</v>
+      </c>
       <c r="E16" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1935,9 +1945,11 @@
       <c r="C17" s="17">
         <v>830</v>
       </c>
-      <c r="D17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="E17" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1954,7 +1966,7 @@
         <v>46</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1962,7 +1974,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>22</v>
@@ -1971,73 +1983,73 @@
         <v>41</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2084,7 +2096,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
@@ -2103,16 +2115,16 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2120,36 +2132,36 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2157,54 +2169,54 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -2212,74 +2224,74 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -2287,10 +2299,10 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
@@ -2298,7 +2310,7 @@
         <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
@@ -2306,36 +2318,36 @@
         <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
@@ -2343,34 +2355,34 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.25">
@@ -2378,100 +2390,100 @@
         <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
         <v>31</v>
@@ -2479,17 +2491,17 @@
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.25">
@@ -2499,82 +2511,82 @@
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.25">
@@ -2584,12 +2596,12 @@
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>